<commit_message>
study_windows_freertos_map: More mappings are added
</commit_message>
<xml_diff>
--- a/windows_freertos_api_mapping.xlsx
+++ b/windows_freertos_api_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\brian\tmpdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C2112-5200-4551-B17D-D5AB0D4464B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E20EB-E03D-4B0C-BF85-1F254374B645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>brian</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{42E9870B-ED03-4625-B06A-B414E1DAB965}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>brian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Task Handle will be returned instead of any ID!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Windows</t>
   </si>
@@ -154,13 +188,40 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>rtos_task_create (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_task_suspend (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_task_resume (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_task_priority_set  (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_task_delete  (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_time_delay_ms (component\os\freertos\os_wrapper\os_wrapper_time.c)</t>
+  </si>
+  <si>
+    <t>rtos_task_handle_get (component\os\freertos\os_wrapper\os_wrapper_task.c)</t>
+  </si>
+  <si>
+    <t>rtos_timer_create (component\os\freertos\os_wrapper\os_wrapper_timer.c)</t>
+  </si>
+  <si>
+    <t>rtos_timer_start (component\os\freertos\os_wrapper\os_wrapper_timer.c)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +252,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +276,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -251,6 +343,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,11 +636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,13 +660,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -603,67 +709,81 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -671,31 +791,37 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -755,5 +881,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
study_windows_freertos_map: Initial completed draft of the function mapping between windows and freeRTOS
</commit_message>
<xml_diff>
--- a/windows_freertos_api_mapping.xlsx
+++ b/windows_freertos_api_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\brian\tmpdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E20EB-E03D-4B0C-BF85-1F254374B645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C829209-136A-4AE9-95C2-A7E78DB1E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>brian</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{42E9870B-ED03-4625-B06A-B414E1DAB965}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{42E9870B-ED03-4625-B06A-B414E1DAB965}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Windows</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>rtos_timer_start (component\os\freertos\os_wrapper\os_wrapper_timer.c)</t>
+  </si>
+  <si>
+    <t>xEventGroupSetBits (component\os\freertos\freertos_v10.4.3\Source\event_groups.c)</t>
+  </si>
+  <si>
+    <t>xEventGroupWaitBits (component\os\freertos\freertos_v10.4.3\Source\event_groups.c)</t>
+  </si>
+  <si>
+    <t>xEventGroupCreate (component\os\freertos\freertos_v10.4.3\Source\event_groups.c)</t>
+  </si>
+  <si>
+    <t>rtos_time_get_current_system_time_ns (component\os\freertos\os_wrapper\os_wrapper_time.c)</t>
   </si>
 </sst>
 </file>
@@ -325,16 +337,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -637,246 +647,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>43</v>
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>44</v>
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>45</v>
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>46</v>
+      <c r="A10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>49</v>
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>48</v>
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>24</v>
+      <c r="A15" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>51</v>
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="A17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>